<commit_message>
change nobles csv and excel file
</commit_message>
<xml_diff>
--- a/resources/config/nobles.xlsx
+++ b/resources/config/nobles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom de Jong labtop\workspace\IIPSEN\resources\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E14C2D4-A020-4CF3-BC8D-56B2A9DF6BB7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{AD870E70-68E7-4F5D-A77B-D012DCE60849}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{1CCBC970-701B-45C6-B92A-9E0A5BC25482}"/>
   </bookViews>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
-  <si>
-    <t>noble</t>
-  </si>
-  <si>
-    <t>Noble</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Diamond</t>
   </si>
@@ -48,9 +42,6 @@
     <t>Onyx</t>
   </si>
   <si>
-    <t>Prestige</t>
-  </si>
-  <si>
     <t>Illustration</t>
   </si>
   <si>
@@ -82,13 +73,16 @@
   </si>
   <si>
     <t>noble9</t>
+  </si>
+  <si>
+    <t>noble10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,12 +95,6 @@
       <color rgb="FF24292E"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF24292E"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -156,13 +144,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -485,27 +470,30 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" t="s">
-        <v>9</v>
+      <c r="B1" t="s">
+        <v>6</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -516,252 +504,184 @@
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1">
-        <v>3</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1">
-        <v>3</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1">
+        <v>3</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3">
-        <v>3</v>
-      </c>
-      <c r="F4" s="3">
-        <v>3</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1"/>
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
       <c r="E5" s="1">
         <v>3</v>
       </c>
-      <c r="F5" s="1">
-        <v>3</v>
-      </c>
-      <c r="G5" s="1">
-        <v>3</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="F5" s="1"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3">
-        <v>4</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2">
         <v>4</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1">
-        <v>4</v>
-      </c>
-      <c r="G7" s="1">
-        <v>4</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3">
-        <v>4</v>
-      </c>
-      <c r="F8" s="3">
-        <v>4</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1">
-        <v>4</v>
-      </c>
-      <c r="H9" s="1">
-        <v>4</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="E9" s="1">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="3">
-        <v>4</v>
-      </c>
-      <c r="E10" s="3">
-        <v>4</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
       <c r="F11" s="1">
         <v>3</v>
       </c>
-      <c r="G11" s="1">
-        <v>3</v>
-      </c>
-      <c r="H11" s="1">
-        <v>3</v>
-      </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3">
-        <v>3</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3">
-        <v>3</v>
-      </c>
-      <c r="H12" s="3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
+      <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>

</xml_diff>